<commit_message>
Add min columns management
</commit_message>
<xml_diff>
--- a/src/main/resources/poi_test.xlsx
+++ b/src/main/resources/poi_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Teste Texto</t>
   </si>
@@ -371,6 +371,57 @@
         <v>43863.0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.121212</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>43861.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>43862.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F11" s="3">
+        <v>43863.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>